<commit_message>
schemas figures et amelioration E2
</commit_message>
<xml_diff>
--- a/projet_E2/Rapport E2/figures/planning_prévisionnel.xlsx
+++ b/projet_E2/Rapport E2/figures/planning_prévisionnel.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="previsionnel" sheetId="1" r:id="rId1"/>
+    <sheet name="reel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Tâches</t>
   </si>
@@ -30,9 +29,6 @@
     <t>Data Science</t>
   </si>
   <si>
-    <t>Rendus</t>
-  </si>
-  <si>
     <t>Rédaction du rapport</t>
   </si>
   <si>
@@ -58,6 +54,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Livrables</t>
   </si>
 </sst>
 </file>
@@ -87,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -110,11 +109,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -123,6 +159,21 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,183 +468,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+    <row r="2" spans="2:12">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3">
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
         <v>45286</v>
       </c>
-      <c r="D1" s="3">
+      <c r="E2" s="3">
         <v>45287</v>
       </c>
-      <c r="E1" s="3">
+      <c r="F2" s="3">
         <v>45288</v>
       </c>
-      <c r="F1" s="3">
+      <c r="G2" s="3">
         <v>45289</v>
       </c>
-      <c r="G1" s="3">
+      <c r="H2" s="3">
         <v>45290</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="2"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="10"/>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="11"/>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="2"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="11"/>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="11"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="10"/>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="H11" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="10"/>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="C15" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -601,24 +661,153 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45286</v>
+      </c>
+      <c r="E2" s="3">
+        <v>45287</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45288</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45289</v>
+      </c>
+      <c r="H2" s="3">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="10"/>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="11"/>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="11"/>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="11"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="10"/>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="10"/>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>